<commit_message>
added new sceanrio and tests
</commit_message>
<xml_diff>
--- a/manual-tests/shopping-test-suite.xlsx
+++ b/manual-tests/shopping-test-suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulwahid/Projects/shoppingElectronTest/manual-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928E3353-74D2-7249-BF1F-9B6F524A9FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1DB195-C2B4-6645-9A7D-683C11A7C0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -403,6 +403,21 @@
   </si>
   <si>
     <t xml:space="preserve">The order should not be submitted, a warning message should appear and warn the user </t>
+  </si>
+  <si>
+    <t>CHECK-004</t>
+  </si>
+  <si>
+    <t>CHECK-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Users fills no details 2)  Click Place Order </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A message will say "Full name is required. A valid email is required. Address is required. City is required. Postcode is required." </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for required fields  </t>
   </si>
 </sst>
 </file>
@@ -774,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScale="162" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="162" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1304,7 +1319,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
         <v>119</v>
@@ -1323,6 +1338,26 @@
       </c>
       <c r="G26" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>